<commit_message>
reorganized files and re-ran calculations
</commit_message>
<xml_diff>
--- a/data_files/miscData/national_income.xlsx
+++ b/data_files/miscData/national_income.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali/DistributionalNationalAccounts-Pakistan/data_files/miscData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A17051F-344B-0541-83A6-D1D33FD0DA3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3472845-2205-294C-8932-68FE7F02CF8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1305,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>